<commit_message>
add schottky diodes and generate prod files
</commit_message>
<xml_diff>
--- a/hardware/kicad/pcbway/BOM_traffic_paradise.xlsx
+++ b/hardware/kicad/pcbway/BOM_traffic_paradise.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bapti\Documents\traffic-pcb-sb\hardware\kicad\pcbway\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D5B572-5ECB-40E4-AC5E-991F1FE01367}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5828485-CA94-4D02-92C5-FCEEFEFA622D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19200" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="155">
   <si>
     <t>xxxx xxxx xxxxx xxPCS BOM  (Sample Bill of Materials)</t>
   </si>
@@ -297,15 +297,9 @@
     <t>6.3V 10uF X5R ±20% 0402 Multilayer Ceramic Capacitors MLCC - SMD/SMT ROHS</t>
   </si>
   <si>
-    <t>LCSC: C17888</t>
-  </si>
-  <si>
     <t>D1,D4</t>
   </si>
   <si>
-    <t>D_SMA</t>
-  </si>
-  <si>
     <t>SW_SPST_SKQG_WithoutStem</t>
   </si>
   <si>
@@ -381,30 +375,6 @@
     <t>62.5mW Thick Film Resistors 50V ±800ppm/℃ ±1% 0Ω 0402 Chip Resistor - Surface Mount ROHS</t>
   </si>
   <si>
-    <t>R10</t>
-  </si>
-  <si>
-    <t>0603WAF1500T5E</t>
-  </si>
-  <si>
-    <t>100mW Thick Film Resistors 75V ±100ppm/℃ ±1% 150Ω 0603 Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
-    <t>LCSC: C22808</t>
-  </si>
-  <si>
-    <t>R137</t>
-  </si>
-  <si>
-    <t>LCSC: C23253</t>
-  </si>
-  <si>
-    <t>0603WAF8200T5E</t>
-  </si>
-  <si>
-    <t>100mW Thick Film Resistors 75V ±100ppm/℃ ±1% 820Ω 0603 Chip Resistor - Surface Mount ROHS</t>
-  </si>
-  <si>
     <t>C3</t>
   </si>
   <si>
@@ -508,13 +478,94 @@
   </si>
   <si>
     <t>LCSC: C10077</t>
+  </si>
+  <si>
+    <t>DIO_RB051MM_ROM</t>
+  </si>
+  <si>
+    <t>Rohm Semiconductor</t>
+  </si>
+  <si>
+    <t>RBR3MM40ATR</t>
+  </si>
+  <si>
+    <t>Diode 40 V 3A Surface Mount PMDU</t>
+  </si>
+  <si>
+    <t>LCSC: C5189742</t>
+  </si>
+  <si>
+    <t>U1</t>
+  </si>
+  <si>
+    <t>LCSC: C627328</t>
+  </si>
+  <si>
+    <t>Microchip Tech</t>
+  </si>
+  <si>
+    <t>MCP4651T-503E/ST</t>
+  </si>
+  <si>
+    <t>±20% I2C 50kΩ 1.8V~5.5V TSSOP-14 Digital Potentiometers ROHS</t>
+  </si>
+  <si>
+    <t>TSSOP-14</t>
+  </si>
+  <si>
+    <t>R1</t>
+  </si>
+  <si>
+    <t>LCSC: C23125</t>
+  </si>
+  <si>
+    <t>0603WAF9091T5E</t>
+  </si>
+  <si>
+    <t>100mW Thick Film Resistors 75V ±100ppm/℃ ±1% 9.09kΩ 0603 Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>R3</t>
+  </si>
+  <si>
+    <t>LCSC: C22874</t>
+  </si>
+  <si>
+    <t>0603WAF1472T5E</t>
+  </si>
+  <si>
+    <t>100mW Thick Film Resistors 75V ±100ppm/℃ ±1% 14.7kΩ 0603 Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>R4</t>
+  </si>
+  <si>
+    <t>0603WAF1501T5E</t>
+  </si>
+  <si>
+    <t>100mW Thick Film Resistors 75V ±100ppm/℃ ±1% 1.5kΩ 0603 Chip Resistor - Surface Mount ROHS</t>
+  </si>
+  <si>
+    <t>LCSC: C22843</t>
+  </si>
+  <si>
+    <t>LCSC: C22908</t>
+  </si>
+  <si>
+    <t>R7</t>
+  </si>
+  <si>
+    <t>0603WAF2491T5E</t>
+  </si>
+  <si>
+    <t>100mW Thick Film Resistors 75V ±100ppm/℃ ±1% 2.49kΩ 0603 Chip Resistor - Surface Mount ROHS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -560,6 +611,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF1C1F23"/>
+      <name val="Poppins SemiBold"/>
     </font>
   </fonts>
   <fills count="4">
@@ -611,7 +667,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -646,6 +702,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -998,10 +1057,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:I31"/>
+  <dimension ref="A2:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E41" sqref="E41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25"/>
@@ -1320,7 +1379,7 @@
         <v>58</v>
       </c>
       <c r="G15" s="10" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>10</v>
@@ -1392,22 +1451,28 @@
         <v>12</v>
       </c>
       <c r="B18" s="10" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C18" s="6">
         <v>2</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
+      <c r="D18" s="7" t="s">
+        <v>129</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>130</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>131</v>
+      </c>
       <c r="G18" s="10" t="s">
-        <v>69</v>
+        <v>128</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I18" s="9" t="s">
-        <v>67</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75">
@@ -1415,28 +1480,28 @@
         <v>13</v>
       </c>
       <c r="B19" s="10" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C19" s="6">
         <v>2</v>
       </c>
       <c r="D19" s="7" t="s">
+        <v>71</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>72</v>
+      </c>
+      <c r="F19" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="E19" s="7" t="s">
+      <c r="G19" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="G19" s="10" t="s">
-        <v>76</v>
-      </c>
       <c r="H19" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I19" s="9" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75">
@@ -1444,7 +1509,7 @@
         <v>14</v>
       </c>
       <c r="B20" s="10" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C20" s="6">
         <v>2</v>
@@ -1453,10 +1518,10 @@
         <v>38</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="G20" s="10" t="s">
         <v>19</v>
@@ -1465,7 +1530,7 @@
         <v>10</v>
       </c>
       <c r="I20" s="9" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15.75">
@@ -1473,7 +1538,7 @@
         <v>15</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C21" s="6">
         <v>2</v>
@@ -1482,10 +1547,10 @@
         <v>38</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G21" s="10" t="s">
         <v>19</v>
@@ -1494,7 +1559,7 @@
         <v>10</v>
       </c>
       <c r="I21" s="9" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75">
@@ -1502,28 +1567,28 @@
         <v>16</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C22" s="6">
         <v>2</v>
       </c>
       <c r="D22" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="F22" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="E22" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>90</v>
-      </c>
       <c r="G22" s="10" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H22" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I22" s="9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75">
@@ -1531,7 +1596,7 @@
         <v>17</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C23" s="6">
         <v>1</v>
@@ -1540,10 +1605,10 @@
         <v>38</v>
       </c>
       <c r="E23" s="7" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="F23" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="G23" s="10" t="s">
         <v>19</v>
@@ -1552,50 +1617,50 @@
         <v>10</v>
       </c>
       <c r="I23" s="9" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75">
       <c r="A24" s="5">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C24" s="6">
         <v>1</v>
       </c>
       <c r="D24" s="7" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E24" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="F24" s="8" t="s">
         <v>96</v>
       </c>
-      <c r="F24" s="8" t="s">
+      <c r="G24" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="G24" s="10" t="s">
-        <v>51</v>
-      </c>
       <c r="H24" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I24" s="9" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75">
       <c r="A25" s="5">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C25" s="6">
         <v>1</v>
       </c>
       <c r="D25" s="7" t="s">
-        <v>38</v>
+        <v>100</v>
       </c>
       <c r="E25" s="7" t="s">
         <v>101</v>
@@ -1604,79 +1669,79 @@
         <v>102</v>
       </c>
       <c r="G25" s="10" t="s">
-        <v>51</v>
+        <v>106</v>
       </c>
       <c r="H25" s="9" t="s">
-        <v>10</v>
+        <v>107</v>
       </c>
       <c r="I25" s="9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="15.75">
       <c r="A26" s="5">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="C26" s="6">
         <v>1</v>
       </c>
       <c r="D26" s="7" t="s">
-        <v>29</v>
+        <v>108</v>
       </c>
       <c r="E26" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="F26" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="G26" s="10" t="s">
         <v>105</v>
       </c>
-      <c r="F26" s="8" t="s">
-        <v>106</v>
-      </c>
-      <c r="G26" s="10" t="s">
-        <v>107</v>
-      </c>
       <c r="H26" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I26" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:9" ht="15.75">
       <c r="A27" s="5">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B27" s="10" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C27" s="6">
         <v>1</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="F27" s="8" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="G27" s="10" t="s">
         <v>116</v>
       </c>
       <c r="H27" s="9" t="s">
-        <v>117</v>
+        <v>10</v>
       </c>
       <c r="I27" s="9" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75">
       <c r="A28" s="5">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="C28" s="6">
         <v>1</v>
@@ -1691,96 +1756,173 @@
         <v>120</v>
       </c>
       <c r="G28" s="10" t="s">
-        <v>115</v>
+        <v>121</v>
       </c>
       <c r="H28" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I28" s="9" t="s">
-        <v>113</v>
-      </c>
+      <c r="I28" s="9"/>
     </row>
     <row r="29" spans="1:9" ht="15.75">
-      <c r="A29" s="5">
-        <v>23</v>
-      </c>
+      <c r="A29" s="5"/>
       <c r="B29" s="10" t="s">
-        <v>121</v>
+        <v>133</v>
       </c>
       <c r="C29" s="6">
         <v>1</v>
       </c>
       <c r="D29" s="7" t="s">
-        <v>123</v>
+        <v>135</v>
       </c>
       <c r="E29" s="7" t="s">
-        <v>124</v>
+        <v>136</v>
       </c>
       <c r="F29" s="8" t="s">
-        <v>125</v>
+        <v>137</v>
       </c>
       <c r="G29" s="10" t="s">
-        <v>126</v>
+        <v>138</v>
       </c>
       <c r="H29" s="9" t="s">
         <v>10</v>
       </c>
       <c r="I29" s="9" t="s">
-        <v>122</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75">
-      <c r="A30" s="5">
-        <v>24</v>
-      </c>
+      <c r="A30" s="5"/>
       <c r="B30" s="10" t="s">
-        <v>127</v>
+        <v>139</v>
       </c>
       <c r="C30" s="6">
         <v>1</v>
       </c>
       <c r="D30" s="7" t="s">
-        <v>128</v>
+        <v>38</v>
       </c>
       <c r="E30" s="7" t="s">
-        <v>129</v>
+        <v>141</v>
       </c>
       <c r="F30" s="8" t="s">
-        <v>130</v>
+        <v>142</v>
       </c>
       <c r="G30" s="10" t="s">
-        <v>131</v>
+        <v>51</v>
       </c>
       <c r="H30" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="I30" s="9"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75">
-      <c r="A31" s="5">
-        <v>25</v>
-      </c>
+      <c r="I30" s="9" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" ht="24" customHeight="1">
+      <c r="A31" s="5"/>
       <c r="B31" s="10" t="s">
-        <v>132</v>
+        <v>143</v>
       </c>
       <c r="C31" s="6">
         <v>1</v>
       </c>
       <c r="D31" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="E31" s="7" t="s">
-        <v>134</v>
+        <v>38</v>
+      </c>
+      <c r="E31" s="13" t="s">
+        <v>145</v>
       </c>
       <c r="F31" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="G31" s="10"/>
+        <v>146</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>51</v>
+      </c>
       <c r="H31" s="9" t="s">
-        <v>136</v>
+        <v>10</v>
       </c>
       <c r="I31" s="9" t="s">
-        <v>137</v>
+        <v>144</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" ht="15.75">
+      <c r="A32" s="5"/>
+      <c r="B32" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="C32" s="6">
+        <v>1</v>
+      </c>
+      <c r="D32" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>148</v>
+      </c>
+      <c r="F32" s="8" t="s">
+        <v>149</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H32" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" ht="15.75">
+      <c r="A33" s="5"/>
+      <c r="B33" s="10" t="s">
+        <v>152</v>
+      </c>
+      <c r="C33" s="6">
+        <v>1</v>
+      </c>
+      <c r="D33" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E33" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F33" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>51</v>
+      </c>
+      <c r="H33" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="15.75">
+      <c r="A34" s="5">
+        <v>25</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>122</v>
+      </c>
+      <c r="C34" s="6">
+        <v>1</v>
+      </c>
+      <c r="D34" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E34" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F34" s="8" t="s">
+        <v>125</v>
+      </c>
+      <c r="G34" s="10"/>
+      <c r="H34" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>